<commit_message>
evento inicio completo 2
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AppointmentLE.xlsx
+++ b/docs/StructureDefinition-AppointmentLE.xlsx
@@ -9,11 +9,14 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$48</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="403">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-17T23:45:39-03:00</t>
+    <t>2023-01-18T13:51:24-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -480,6 +483,206 @@
     <t>SCH-1, SCH-2, ARQ-1, ARQ-2</t>
   </si>
   <si>
+    <t>Appointment.identifier.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string
+</t>
+  </si>
+  <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.use</t>
+  </si>
+  <si>
+    <t>usual | official | temp | secondary | old (If known)</t>
+  </si>
+  <si>
+    <t>The purpose of this identifier.</t>
+  </si>
+  <si>
+    <t>Applications can assume that an identifier is permanent unless it explicitly says that it is temporary.</t>
+  </si>
+  <si>
+    <t>Allows the appropriate identifier for a particular context of use to be selected from among a set of identifiers.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Identifies the purpose for this identifier, if known .</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-use|4.0.1</t>
+  </si>
+  <si>
+    <t>Identifier.use</t>
+  </si>
+  <si>
+    <t>Role.code or implied by context</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeableConcept
+</t>
+  </si>
+  <si>
+    <t>Description of identifier</t>
+  </si>
+  <si>
+    <t>A coded type for the identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>This element deals only with general categories of identifiers.  It SHOULD not be used for codes that correspond 1..1 with the Identifier.system. Some identifiers may fall into multiple categories due to common usage.   Where the system is known, a type is unnecessary because the type is always part of the system definition. However systems often need to handle identifiers where the system is not known. There is not a 1:1 relationship between type and system, since many different systems have the same type.</t>
+  </si>
+  <si>
+    <t>Allows users to make use of identifiers when the identifier system is not known.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+  </si>
+  <si>
+    <t>Identifier.type</t>
+  </si>
+  <si>
+    <t>CX.5</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.system</t>
+  </si>
+  <si>
+    <t>The namespace for the identifier value</t>
+  </si>
+  <si>
+    <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
+  </si>
+  <si>
+    <t>Identifier.system is always case sensitive.</t>
+  </si>
+  <si>
+    <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
+  </si>
+  <si>
+    <t>http://www.acme.com/identifiers/patient</t>
+  </si>
+  <si>
+    <t>Identifier.system</t>
+  </si>
+  <si>
+    <t>II.root or Role.id.root</t>
+  </si>
+  <si>
+    <t>CX.4 / EI-2-4</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.value</t>
+  </si>
+  <si>
+    <t>The value that is unique</t>
+  </si>
+  <si>
+    <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
+  </si>
+  <si>
+    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://hl7.org/fhir/R4/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>Identifier.value</t>
+  </si>
+  <si>
+    <t>II.extension or II.root if system indicates OID or GUID (Or Role.id.extension or root)</t>
+  </si>
+  <si>
+    <t>CX.1 / EI.1</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period
+</t>
+  </si>
+  <si>
+    <t>Time period when id is/was valid for use</t>
+  </si>
+  <si>
+    <t>Time period during which identifier is/was valid for use.</t>
+  </si>
+  <si>
+    <t>Identifier.period</t>
+  </si>
+  <si>
+    <t>Role.effectiveTime or implied by context</t>
+  </si>
+  <si>
+    <t>CX.7 + CX.8</t>
+  </si>
+  <si>
+    <t>Appointment.identifier.assigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Organization)
+</t>
+  </si>
+  <si>
+    <t>Organization that issued id (may be just text)</t>
+  </si>
+  <si>
+    <t>Organization that issued/manages the identifier.</t>
+  </si>
+  <si>
+    <t>The Identifier.assigner may omit the .reference element and only contain a .display element reflecting the name or other textual information about the assigning organization.</t>
+  </si>
+  <si>
+    <t>Identifier.assigner</t>
+  </si>
+  <si>
+    <t>II.assigningAuthorityName but note that this is an improper use by the definition of the field.  Also Role.scoper</t>
+  </si>
+  <si>
+    <t>CX.4 / (CX.4,CX.9,CX.10)</t>
+  </si>
+  <si>
     <t>Appointment.status</t>
   </si>
   <si>
@@ -493,7 +696,7 @@
 This element is labeled as a modifier because the status contains the code entered-in-error that mark the Appointment as not currently valid.</t>
   </si>
   <si>
-    <t>required</t>
+    <t>booked</t>
   </si>
   <si>
     <t>The free/busy status of an appointment.</t>
@@ -520,10 +723,6 @@
     <t>Appointment.cancelationReason</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept
-</t>
-  </si>
-  <si>
     <t>The coded reason for the appointment being cancelled</t>
   </si>
   <si>
@@ -534,9 +733,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/appointment-cancellation-reason</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Appointment.serviceCategory</t>
@@ -690,10 +886,6 @@
     <t>Appointment.description</t>
   </si>
   <si>
-    <t xml:space="preserve">string
-</t>
-  </si>
-  <si>
     <t>Shown on a subject line in a meeting request, or appointment list</t>
   </si>
   <si>
@@ -933,22 +1125,7 @@
     <t>Appointment.participant.id</t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
     <t>Appointment.participant.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Appointment.participant.modifierExtension</t>
@@ -984,9 +1161,6 @@
 This value SHALL be the same when creating an AppointmentResponse so that they can be matched, and subsequently update the Appointment.</t>
   </si>
   <si>
-    <t>extensible</t>
-  </si>
-  <si>
     <t>Role of participant in encounter.</t>
   </si>
   <si>
@@ -1070,10 +1244,6 @@
   </si>
   <si>
     <t>Appointment.participant.period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period
-</t>
   </si>
   <si>
     <t>Participation period of the actor</t>
@@ -1227,6 +1397,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1395,7 +1580,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO40"/>
+  <dimension ref="A1:AO48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1423,16 +1608,16 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="38.8125" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="49.39453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="95.56640625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="56.84765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.8203125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1571,7 +1756,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>26</v>
       </c>
@@ -1686,7 +1871,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>83</v>
       </c>
@@ -1803,7 +1988,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>91</v>
       </c>
@@ -1918,7 +2103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>97</v>
       </c>
@@ -2035,7 +2220,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>103</v>
       </c>
@@ -2152,7 +2337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>112</v>
       </c>
@@ -2269,7 +2454,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>120</v>
       </c>
@@ -2386,7 +2571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>128</v>
       </c>
@@ -2503,7 +2688,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>136</v>
       </c>
@@ -2622,7 +2807,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>141</v>
       </c>
@@ -2635,13 +2820,13 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>74</v>
@@ -2737,7 +2922,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>150</v>
       </c>
@@ -2750,7 +2935,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>84</v>
@@ -2759,23 +2944,21 @@
         <v>74</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="N12" t="s" s="2">
         <v>153</v>
       </c>
+      <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" t="s" s="2">
         <v>74</v>
@@ -2800,34 +2983,34 @@
         <v>74</v>
       </c>
       <c r="X12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE12" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF12" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="Y12" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="Z12" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="AA12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AB12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AD12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AE12" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AF12" t="s" s="2">
-        <v>150</v>
-      </c>
       <c r="AG12" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>84</v>
@@ -2836,41 +3019,41 @@
         <v>74</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>157</v>
+        <v>74</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="AO12" t="s" s="2">
-        <v>161</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>74</v>
@@ -2879,18 +3062,20 @@
         <v>74</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="N13" t="s" s="2">
+        <v>133</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
         <v>74</v>
@@ -2915,64 +3100,66 @@
         <v>74</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="Y13" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="Y13" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="Z13" t="s" s="2">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="AA13" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>74</v>
+        <v>158</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="AD13" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="AF13" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG13" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH13" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ13" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AK13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL13" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN13" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO13" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" hidden="true">
+      <c r="A14" t="s" s="2">
         <v>162</v>
       </c>
-      <c r="AG13" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AH13" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ13" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="AK13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AL13" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AM13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AN13" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AO13" t="s" s="2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>169</v>
-      </c>
       <c r="B14" t="s" s="2">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -2983,28 +3170,32 @@
         <v>75</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J14" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K14" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L14" t="s" s="2">
         <v>163</v>
       </c>
-      <c r="L14" t="s" s="2">
-        <v>170</v>
-      </c>
       <c r="M14" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="O14" t="s" s="2">
+        <v>166</v>
+      </c>
       <c r="P14" t="s" s="2">
         <v>74</v>
       </c>
@@ -3028,11 +3219,13 @@
         <v>74</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="Y14" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="Y14" t="s" s="2">
+        <v>168</v>
+      </c>
       <c r="Z14" t="s" s="2">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>74</v>
@@ -3050,13 +3243,13 @@
         <v>74</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>74</v>
@@ -3068,24 +3261,24 @@
         <v>74</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>174</v>
+        <v>74</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO14" t="s" s="2">
-        <v>74</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3096,7 +3289,7 @@
         <v>75</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>74</v>
@@ -3108,18 +3301,20 @@
         <v>85</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="L15" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="N15" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="M15" t="s" s="2">
+      <c r="O15" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="N15" t="s" s="2">
-        <v>178</v>
-      </c>
-      <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
         <v>74</v>
       </c>
@@ -3143,11 +3338,13 @@
         <v>74</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="Y15" s="2"/>
+        <v>178</v>
+      </c>
+      <c r="Y15" t="s" s="2">
+        <v>179</v>
+      </c>
       <c r="Z15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>74</v>
@@ -3165,13 +3362,13 @@
         <v>74</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>74</v>
@@ -3180,10 +3377,10 @@
         <v>96</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>74</v>
@@ -3192,15 +3389,15 @@
         <v>74</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>74</v>
+        <v>182</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3208,13 +3405,13 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>74</v>
@@ -3223,16 +3420,20 @@
         <v>85</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+        <v>185</v>
+      </c>
+      <c r="N16" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="O16" t="s" s="2">
+        <v>187</v>
+      </c>
       <c r="P16" t="s" s="2">
         <v>74</v>
       </c>
@@ -3244,7 +3445,7 @@
         <v>74</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>74</v>
+        <v>188</v>
       </c>
       <c r="U16" t="s" s="2">
         <v>74</v>
@@ -3256,11 +3457,13 @@
         <v>74</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="Y16" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="Y16" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="Z16" t="s" s="2">
-        <v>184</v>
+        <v>74</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>74</v>
@@ -3278,13 +3481,13 @@
         <v>74</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>74</v>
@@ -3296,24 +3499,24 @@
         <v>74</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>186</v>
+        <v>74</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>74</v>
+        <v>191</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3321,13 +3524,13 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>74</v>
@@ -3336,15 +3539,17 @@
         <v>85</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="N17" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="N17" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
         <v>74</v>
@@ -3357,7 +3562,7 @@
         <v>74</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>74</v>
@@ -3369,11 +3574,13 @@
         <v>74</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="Y17" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="Y17" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="Z17" t="s" s="2">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>74</v>
@@ -3391,7 +3598,7 @@
         <v>74</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>75</v>
@@ -3409,24 +3616,24 @@
         <v>74</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>192</v>
+        <v>74</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3437,7 +3644,7 @@
         <v>75</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>74</v>
@@ -3449,13 +3656,13 @@
         <v>85</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3482,13 +3689,13 @@
         <v>74</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>197</v>
+        <v>74</v>
       </c>
       <c r="Z18" t="s" s="2">
-        <v>198</v>
+        <v>74</v>
       </c>
       <c r="AA18" t="s" s="2">
         <v>74</v>
@@ -3506,13 +3713,13 @@
         <v>74</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>74</v>
@@ -3521,10 +3728,10 @@
         <v>96</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>199</v>
+        <v>74</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>74</v>
@@ -3533,15 +3740,15 @@
         <v>74</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3552,7 +3759,7 @@
         <v>75</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>74</v>
@@ -3561,18 +3768,20 @@
         <v>74</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>210</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>211</v>
+      </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
         <v>74</v>
@@ -3621,13 +3830,13 @@
         <v>74</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI19" t="s" s="2">
         <v>74</v>
@@ -3636,10 +3845,10 @@
         <v>96</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>206</v>
+        <v>74</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>74</v>
@@ -3648,15 +3857,15 @@
         <v>74</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>74</v>
+        <v>214</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3664,31 +3873,31 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>209</v>
+        <v>104</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
@@ -3699,7 +3908,7 @@
         <v>74</v>
       </c>
       <c r="S20" t="s" s="2">
-        <v>74</v>
+        <v>219</v>
       </c>
       <c r="T20" t="s" s="2">
         <v>74</v>
@@ -3714,13 +3923,13 @@
         <v>74</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>74</v>
+        <v>167</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>74</v>
+        <v>221</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>74</v>
@@ -3738,10 +3947,10 @@
         <v>74</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>84</v>
@@ -3753,27 +3962,27 @@
         <v>96</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3793,16 +4002,16 @@
         <v>74</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -3829,13 +4038,11 @@
         <v>74</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y21" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y21" s="2"/>
       <c r="Z21" t="s" s="2">
-        <v>74</v>
+        <v>231</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>74</v>
@@ -3853,7 +4060,7 @@
         <v>74</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>75</v>
@@ -3871,24 +4078,24 @@
         <v>74</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>221</v>
+        <v>155</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>223</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3908,16 +4115,16 @@
         <v>74</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>225</v>
+        <v>173</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -3944,13 +4151,11 @@
         <v>74</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y22" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y22" s="2"/>
       <c r="Z22" t="s" s="2">
-        <v>74</v>
+        <v>235</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>74</v>
@@ -3968,7 +4173,7 @@
         <v>74</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>75</v>
@@ -3983,27 +4188,27 @@
         <v>96</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>228</v>
+        <v>74</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4014,7 +4219,7 @@
         <v>75</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>74</v>
@@ -4026,15 +4231,17 @@
         <v>85</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>233</v>
+        <v>173</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N23" s="2"/>
+        <v>240</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>241</v>
+      </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
         <v>74</v>
@@ -4059,13 +4266,11 @@
         <v>74</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y23" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
-        <v>74</v>
+        <v>242</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>74</v>
@@ -4083,13 +4288,13 @@
         <v>74</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>74</v>
@@ -4098,27 +4303,27 @@
         <v>96</v>
       </c>
       <c r="AK23" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="AL23" t="s" s="2">
         <v>236</v>
       </c>
-      <c r="AL23" t="s" s="2">
-        <v>237</v>
-      </c>
       <c r="AM23" t="s" s="2">
-        <v>238</v>
+        <v>74</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>239</v>
+        <v>74</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>240</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4129,7 +4334,7 @@
         <v>75</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>74</v>
@@ -4141,13 +4346,13 @@
         <v>85</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>233</v>
+        <v>173</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4174,13 +4379,11 @@
         <v>74</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y24" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="Y24" s="2"/>
       <c r="Z24" t="s" s="2">
-        <v>74</v>
+        <v>247</v>
       </c>
       <c r="AA24" t="s" s="2">
         <v>74</v>
@@ -4198,13 +4401,13 @@
         <v>74</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>74</v>
@@ -4213,27 +4416,27 @@
         <v>96</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>236</v>
+        <v>74</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>245</v>
+        <v>74</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>247</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4253,16 +4456,16 @@
         <v>74</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -4289,13 +4492,11 @@
         <v>74</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y25" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="Y25" s="2"/>
       <c r="Z25" t="s" s="2">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>74</v>
@@ -4313,7 +4514,7 @@
         <v>74</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>75</v>
@@ -4328,27 +4529,27 @@
         <v>96</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>236</v>
+        <v>74</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>74</v>
+        <v>256</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4368,16 +4569,16 @@
         <v>74</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>255</v>
+        <v>173</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4404,13 +4605,13 @@
         <v>74</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>74</v>
+        <v>260</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>74</v>
+        <v>261</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>74</v>
@@ -4428,7 +4629,7 @@
         <v>74</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>75</v>
@@ -4443,10 +4644,10 @@
         <v>96</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>74</v>
+        <v>262</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>74</v>
@@ -4455,15 +4656,15 @@
         <v>74</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>74</v>
+        <v>264</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4474,7 +4675,7 @@
         <v>75</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>74</v>
@@ -4486,17 +4687,15 @@
         <v>74</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>263</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
         <v>74</v>
@@ -4545,13 +4744,13 @@
         <v>74</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>74</v>
@@ -4560,13 +4759,13 @@
         <v>96</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>266</v>
+        <v>74</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>74</v>
@@ -4575,12 +4774,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4603,16 +4802,16 @@
         <v>74</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>218</v>
+        <v>272</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4662,7 +4861,7 @@
         <v>74</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>75</v>
@@ -4677,27 +4876,27 @@
         <v>96</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>74</v>
+        <v>249</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>223</v>
+        <v>279</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4720,13 +4919,13 @@
         <v>74</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>218</v>
+        <v>151</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4777,7 +4976,7 @@
         <v>74</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>75</v>
@@ -4795,28 +4994,28 @@
         <v>74</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>223</v>
+        <v>285</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
-        <v>279</v>
+        <v>74</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s" s="2">
@@ -4835,13 +5034,13 @@
         <v>74</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4892,7 +5091,7 @@
         <v>74</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>75</v>
@@ -4907,27 +5106,27 @@
         <v>96</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>74</v>
+        <v>292</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>74</v>
+        <v>293</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4938,25 +5137,25 @@
         <v>84</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5007,42 +5206,42 @@
         <v>74</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="AG31" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH31" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="AH31" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="AI31" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>289</v>
+        <v>96</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>74</v>
+        <v>301</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>293</v>
+        <v>302</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5062,16 +5261,16 @@
         <v>74</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>218</v>
+        <v>295</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5122,7 +5321,7 @@
         <v>74</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>75</v>
@@ -5134,41 +5333,41 @@
         <v>74</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>74</v>
+        <v>298</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>168</v>
+        <v>306</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>74</v>
+        <v>307</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>74</v>
+        <v>308</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>74</v>
+        <v>309</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>74</v>
@@ -5180,17 +5379,15 @@
         <v>74</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>130</v>
+        <v>311</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>131</v>
+        <v>312</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>133</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
         <v>74</v>
@@ -5239,28 +5436,28 @@
         <v>74</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI33" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>74</v>
+        <v>298</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>168</v>
+        <v>314</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>74</v>
+        <v>315</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>74</v>
@@ -5269,16 +5466,16 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>302</v>
+        <v>74</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -5291,26 +5488,22 @@
         <v>74</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>130</v>
+        <v>317</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="O34" t="s" s="2">
-        <v>139</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
         <v>74</v>
       </c>
@@ -5358,7 +5551,7 @@
         <v>74</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>75</v>
@@ -5370,13 +5563,13 @@
         <v>74</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>127</v>
+        <v>320</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>74</v>
@@ -5388,12 +5581,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5404,7 +5597,7 @@
         <v>75</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>74</v>
@@ -5413,19 +5606,19 @@
         <v>74</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>163</v>
+        <v>322</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>309</v>
+        <v>325</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5451,13 +5644,13 @@
         <v>74</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>310</v>
+        <v>74</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>311</v>
+        <v>74</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>312</v>
+        <v>74</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>74</v>
@@ -5475,13 +5668,13 @@
         <v>74</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI35" t="s" s="2">
         <v>74</v>
@@ -5490,27 +5683,27 @@
         <v>96</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>74</v>
+        <v>326</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>168</v>
+        <v>328</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO35" t="s" s="2">
-        <v>314</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5530,18 +5723,20 @@
         <v>74</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>316</v>
+        <v>151</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>317</v>
+        <v>330</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="N36" s="2"/>
+        <v>331</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>332</v>
+      </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
         <v>74</v>
@@ -5590,7 +5785,7 @@
         <v>74</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>75</v>
@@ -5605,27 +5800,27 @@
         <v>96</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>74</v>
+        <v>333</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>321</v>
+        <v>74</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>322</v>
+        <v>285</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5645,16 +5840,16 @@
         <v>74</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>324</v>
+        <v>337</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>325</v>
+        <v>338</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5681,13 +5876,13 @@
         <v>74</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>326</v>
+        <v>74</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>327</v>
+        <v>74</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>74</v>
@@ -5705,7 +5900,7 @@
         <v>74</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>75</v>
@@ -5723,35 +5918,35 @@
         <v>74</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>74</v>
+        <v>285</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>74</v>
+        <v>341</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>74</v>
@@ -5760,16 +5955,16 @@
         <v>74</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>104</v>
+        <v>342</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5796,13 +5991,13 @@
         <v>74</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>154</v>
+        <v>74</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>333</v>
+        <v>74</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>334</v>
+        <v>74</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>74</v>
@@ -5820,13 +6015,13 @@
         <v>74</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>74</v>
@@ -5835,27 +6030,27 @@
         <v>96</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>74</v>
+        <v>345</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>336</v>
+        <v>74</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>337</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5863,10 +6058,10 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>74</v>
@@ -5878,13 +6073,13 @@
         <v>74</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5935,42 +6130,42 @@
         <v>74</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>96</v>
+        <v>351</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>74</v>
+        <v>352</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>168</v>
+        <v>353</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>74</v>
+        <v>354</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>74</v>
+        <v>355</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>342</v>
+        <v>356</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5981,7 +6176,7 @@
         <v>75</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>74</v>
@@ -5993,17 +6188,15 @@
         <v>74</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>339</v>
+        <v>151</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>343</v>
+        <v>152</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>345</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>74</v>
@@ -6052,37 +6245,985 @@
         <v>74</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>342</v>
+        <v>154</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH40" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL40" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN40" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO40" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G41" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="AI40" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
+      <c r="H41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="O41" s="2"/>
+      <c r="P41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q41" s="2"/>
+      <c r="R41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO41" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>360</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="O42" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="P42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL42" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="AM42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN42" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO42" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" hidden="true">
+      <c r="A43" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G43" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J43" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K43" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q43" s="2"/>
+      <c r="R43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X43" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="AK40" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="AM40" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AN40" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AO40" t="s" s="2">
-        <v>347</v>
+      <c r="AK43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL43" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="AM43" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AN43" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO43" t="s" s="2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="44" hidden="true">
+      <c r="A44" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G44" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J44" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="L44" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>374</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q44" s="2"/>
+      <c r="R44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL44" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AM44" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AN44" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AO44" t="s" s="2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="45" hidden="true">
+      <c r="A45" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q45" s="2"/>
+      <c r="R45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF45" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AG45" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH45" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ45" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL45" t="s" s="2">
+        <v>384</v>
+      </c>
+      <c r="AM45" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="AN45" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO45" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" hidden="true">
+      <c r="A46" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G46" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J46" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L46" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="M46" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q46" s="2"/>
+      <c r="R46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X46" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="Y46" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="Z46" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="AA46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF46" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AG46" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH46" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ46" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL46" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AM46" t="s" s="2">
+        <v>392</v>
+      </c>
+      <c r="AN46" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO46" t="s" s="2">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" hidden="true">
+      <c r="A47" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G47" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K47" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="M47" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q47" s="2"/>
+      <c r="R47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF47" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="AG47" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH47" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ47" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL47" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO47" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" hidden="true">
+      <c r="A48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="B48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="L48" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q48" s="2"/>
+      <c r="R48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF48" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AG48" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ48" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK48" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="AL48" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO48" t="s" s="2">
+        <v>402</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AO48">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI47">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
todos los eventos OK
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-AppointmentLE.xlsx
+++ b/docs/StructureDefinition-AppointmentLE.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$50</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="411">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-19T11:18:06-03:00</t>
+    <t>2023-01-20T14:40:00-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -415,33 +415,61 @@
     <t>Appointment.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>Appointment.extension:MedioNotificacion</t>
+  </si>
+  <si>
+    <t>MedioNotificacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://minsal.cl/listaespera/StructureDefinition/MedioNotificacion}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>Appointment.extension:Contactado</t>
+  </si>
+  <si>
+    <t>Contactado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://minsal.cl/listaespera/StructureDefinition/Contactado}
+</t>
+  </si>
+  <si>
+    <t>Appointment.modifierExtension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Appointment.modifierExtension</t>
-  </si>
-  <si>
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
@@ -449,6 +477,9 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
     <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
@@ -505,17 +536,13 @@
     <t>Appointment.identifier.extension</t>
   </si>
   <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
   </si>
   <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
     <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>Element.extension</t>
@@ -1580,7 +1607,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO48"/>
+  <dimension ref="A1:AO50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1591,7 +1618,7 @@
   <cols>
     <col min="1" max="1" width="40.10546875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="40.10546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.1328125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="17.56640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -2580,11 +2607,11 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s" s="2">
         <v>76</v>
@@ -2599,17 +2626,15 @@
         <v>74</v>
       </c>
       <c r="K9" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="L9" t="s" s="2">
         <v>130</v>
       </c>
-      <c r="L9" t="s" s="2">
+      <c r="M9" t="s" s="2">
         <v>131</v>
       </c>
-      <c r="M9" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="N9" t="s" s="2">
-        <v>133</v>
-      </c>
+      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" t="s" s="2">
         <v>74</v>
@@ -2646,16 +2671,14 @@
         <v>74</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC9" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="AC9" s="2"/>
       <c r="AD9" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>134</v>
@@ -2676,7 +2699,7 @@
         <v>74</v>
       </c>
       <c r="AL9" t="s" s="2">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="AM9" t="s" s="2">
         <v>74</v>
@@ -2693,43 +2716,41 @@
         <v>136</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>137</v>
+      </c>
       <c r="D10" t="s" s="2">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s" s="2">
         <v>74</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="L10" t="s" s="2">
         <v>137</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="O10" t="s" s="2">
-        <v>139</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
       <c r="P10" t="s" s="2">
         <v>74</v>
       </c>
@@ -2777,7 +2798,7 @@
         <v>74</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>75</v>
@@ -2786,7 +2807,7 @@
         <v>76</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>135</v>
@@ -2795,7 +2816,7 @@
         <v>74</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="AM10" t="s" s="2">
         <v>74</v>
@@ -2809,12 +2830,14 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="B11" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
         <v>74</v>
       </c>
@@ -2832,16 +2855,16 @@
         <v>74</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>142</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2892,7 +2915,7 @@
         <v>74</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>75</v>
@@ -2901,65 +2924,69 @@
         <v>76</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>147</v>
+        <v>74</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="AO11" t="s" s="2">
-        <v>149</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s" s="2">
         <v>74</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+        <v>146</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="O12" t="s" s="2">
+        <v>148</v>
+      </c>
       <c r="P12" t="s" s="2">
         <v>74</v>
       </c>
@@ -3007,25 +3034,25 @@
         <v>74</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="AM12" t="s" s="2">
         <v>74</v>
@@ -3039,43 +3066,41 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>133</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
         <v>74</v>
@@ -3112,19 +3137,19 @@
         <v>74</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>158</v>
+        <v>74</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>159</v>
+        <v>74</v>
       </c>
       <c r="AD13" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>160</v>
+        <v>74</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>75</v>
@@ -3136,30 +3161,30 @@
         <v>74</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>74</v>
+        <v>154</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>155</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>74</v>
+        <v>156</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>74</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3176,26 +3201,22 @@
         <v>74</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>104</v>
+        <v>160</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="O14" t="s" s="2">
-        <v>166</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
         <v>74</v>
       </c>
@@ -3219,13 +3240,13 @@
         <v>74</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>168</v>
+        <v>74</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>169</v>
+        <v>74</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>74</v>
@@ -3243,7 +3264,7 @@
         <v>74</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>75</v>
@@ -3255,13 +3276,13 @@
         <v>74</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>74</v>
@@ -3270,26 +3291,26 @@
         <v>74</v>
       </c>
       <c r="AO14" t="s" s="2">
-        <v>127</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>74</v>
@@ -3298,23 +3319,21 @@
         <v>74</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="O15" t="s" s="2">
-        <v>177</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
         <v>74</v>
       </c>
@@ -3338,49 +3357,49 @@
         <v>74</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>179</v>
+        <v>74</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="AC15" t="s" s="2">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="AD15" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>74</v>
@@ -3389,15 +3408,15 @@
         <v>74</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>182</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3405,34 +3424,34 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I16" t="s" s="2">
         <v>85</v>
-      </c>
-      <c r="I16" t="s" s="2">
-        <v>74</v>
       </c>
       <c r="J16" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>74</v>
@@ -3445,7 +3464,7 @@
         <v>74</v>
       </c>
       <c r="T16" t="s" s="2">
-        <v>188</v>
+        <v>74</v>
       </c>
       <c r="U16" t="s" s="2">
         <v>74</v>
@@ -3457,13 +3476,13 @@
         <v>74</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>74</v>
@@ -3481,7 +3500,7 @@
         <v>74</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>75</v>
@@ -3499,7 +3518,7 @@
         <v>74</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>74</v>
@@ -3508,15 +3527,15 @@
         <v>74</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>191</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3524,13 +3543,13 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>74</v>
@@ -3539,18 +3558,20 @@
         <v>85</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="O17" s="2"/>
+        <v>184</v>
+      </c>
+      <c r="O17" t="s" s="2">
+        <v>185</v>
+      </c>
       <c r="P17" t="s" s="2">
         <v>74</v>
       </c>
@@ -3562,7 +3583,7 @@
         <v>74</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>196</v>
+        <v>74</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>74</v>
@@ -3574,13 +3595,13 @@
         <v>74</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>74</v>
+        <v>187</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>74</v>
+        <v>188</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>74</v>
@@ -3598,7 +3619,7 @@
         <v>74</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>75</v>
@@ -3616,7 +3637,7 @@
         <v>74</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>74</v>
@@ -3625,15 +3646,15 @@
         <v>74</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3656,16 +3677,20 @@
         <v>85</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>201</v>
+        <v>98</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="N18" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="O18" t="s" s="2">
+        <v>195</v>
+      </c>
       <c r="P18" t="s" s="2">
         <v>74</v>
       </c>
@@ -3677,7 +3702,7 @@
         <v>74</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="U18" t="s" s="2">
         <v>74</v>
@@ -3713,7 +3738,7 @@
         <v>74</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>75</v>
@@ -3731,7 +3756,7 @@
         <v>74</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="AM18" t="s" s="2">
         <v>74</v>
@@ -3740,15 +3765,15 @@
         <v>74</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3756,13 +3781,13 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>74</v>
@@ -3771,16 +3796,16 @@
         <v>85</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -3794,7 +3819,7 @@
         <v>74</v>
       </c>
       <c r="T19" t="s" s="2">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="U19" t="s" s="2">
         <v>74</v>
@@ -3830,7 +3855,7 @@
         <v>74</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>75</v>
@@ -3848,7 +3873,7 @@
         <v>74</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="AM19" t="s" s="2">
         <v>74</v>
@@ -3857,15 +3882,15 @@
         <v>74</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3873,32 +3898,30 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J20" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>218</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>74</v>
@@ -3908,7 +3931,7 @@
         <v>74</v>
       </c>
       <c r="S20" t="s" s="2">
-        <v>219</v>
+        <v>74</v>
       </c>
       <c r="T20" t="s" s="2">
         <v>74</v>
@@ -3923,13 +3946,13 @@
         <v>74</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>220</v>
+        <v>74</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>221</v>
+        <v>74</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>74</v>
@@ -3947,10 +3970,10 @@
         <v>74</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>84</v>
@@ -3962,27 +3985,27 @@
         <v>96</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>224</v>
+        <v>74</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>225</v>
+        <v>74</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4005,15 +4028,17 @@
         <v>85</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>173</v>
+        <v>216</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>218</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>219</v>
+      </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
         <v>74</v>
@@ -4038,11 +4063,13 @@
         <v>74</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="Y21" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="Y21" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="Z21" t="s" s="2">
-        <v>231</v>
+        <v>74</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>74</v>
@@ -4060,7 +4087,7 @@
         <v>74</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>75</v>
@@ -4078,7 +4105,7 @@
         <v>74</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>155</v>
+        <v>221</v>
       </c>
       <c r="AM21" t="s" s="2">
         <v>74</v>
@@ -4087,15 +4114,15 @@
         <v>74</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>74</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4103,30 +4130,32 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>225</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>226</v>
+      </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
         <v>74</v>
@@ -4136,7 +4165,7 @@
         <v>74</v>
       </c>
       <c r="S22" t="s" s="2">
-        <v>74</v>
+        <v>227</v>
       </c>
       <c r="T22" t="s" s="2">
         <v>74</v>
@@ -4151,11 +4180,13 @@
         <v>74</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="Y22" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="Y22" t="s" s="2">
+        <v>228</v>
+      </c>
       <c r="Z22" t="s" s="2">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="AA22" t="s" s="2">
         <v>74</v>
@@ -4173,13 +4204,13 @@
         <v>74</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>74</v>
@@ -4188,27 +4219,27 @@
         <v>96</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>74</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4219,7 +4250,7 @@
         <v>75</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>74</v>
@@ -4231,17 +4262,15 @@
         <v>85</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>241</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
         <v>74</v>
@@ -4266,11 +4295,11 @@
         <v>74</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="Y23" s="2"/>
       <c r="Z23" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AA23" t="s" s="2">
         <v>74</v>
@@ -4288,13 +4317,13 @@
         <v>74</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>74</v>
@@ -4303,10 +4332,10 @@
         <v>96</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>243</v>
+        <v>74</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>236</v>
+        <v>164</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>74</v>
@@ -4320,10 +4349,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4346,13 +4375,13 @@
         <v>85</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4379,11 +4408,11 @@
         <v>74</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="Y24" s="2"/>
       <c r="Z24" t="s" s="2">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AA24" t="s" s="2">
         <v>74</v>
@@ -4401,7 +4430,7 @@
         <v>74</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>75</v>
@@ -4419,13 +4448,13 @@
         <v>74</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>249</v>
+        <v>74</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>74</v>
@@ -4433,10 +4462,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4447,7 +4476,7 @@
         <v>75</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>74</v>
@@ -4459,15 +4488,17 @@
         <v>85</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N25" s="2"/>
+        <v>248</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>249</v>
+      </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
         <v>74</v>
@@ -4492,11 +4523,11 @@
         <v>74</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>108</v>
+        <v>238</v>
       </c>
       <c r="Y25" s="2"/>
       <c r="Z25" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>74</v>
@@ -4514,13 +4545,13 @@
         <v>74</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>74</v>
@@ -4529,27 +4560,27 @@
         <v>96</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>74</v>
+        <v>251</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>255</v>
+        <v>74</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>256</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4572,13 +4603,13 @@
         <v>85</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
@@ -4607,11 +4638,9 @@
       <c r="X26" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="Y26" t="s" s="2">
-        <v>260</v>
-      </c>
+      <c r="Y26" s="2"/>
       <c r="Z26" t="s" s="2">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>74</v>
@@ -4629,7 +4658,7 @@
         <v>74</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>75</v>
@@ -4644,27 +4673,27 @@
         <v>96</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>262</v>
+        <v>74</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="AM26" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>74</v>
+        <v>257</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>264</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4675,7 +4704,7 @@
         <v>75</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>74</v>
@@ -4684,16 +4713,16 @@
         <v>74</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>266</v>
+        <v>181</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4720,13 +4749,11 @@
         <v>74</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="Y27" s="2"/>
       <c r="Z27" t="s" s="2">
-        <v>74</v>
+        <v>261</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>74</v>
@@ -4744,13 +4771,13 @@
         <v>74</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>74</v>
@@ -4759,27 +4786,27 @@
         <v>96</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>269</v>
+        <v>74</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>74</v>
+        <v>263</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>74</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4790,7 +4817,7 @@
         <v>75</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>74</v>
@@ -4799,20 +4826,18 @@
         <v>74</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>272</v>
+        <v>181</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>275</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>74</v>
@@ -4837,13 +4862,13 @@
         <v>74</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>74</v>
+        <v>268</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>74</v>
+        <v>269</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>74</v>
@@ -4861,13 +4886,13 @@
         <v>74</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>74</v>
@@ -4876,27 +4901,27 @@
         <v>96</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>278</v>
+        <v>74</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>249</v>
+        <v>74</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4907,7 +4932,7 @@
         <v>75</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>74</v>
@@ -4919,13 +4944,13 @@
         <v>74</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>151</v>
+        <v>274</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -4976,13 +5001,13 @@
         <v>74</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>74</v>
@@ -4991,27 +5016,27 @@
         <v>96</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>74</v>
+        <v>277</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>284</v>
+        <v>74</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>285</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5022,7 +5047,7 @@
         <v>75</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>74</v>
@@ -5034,15 +5059,17 @@
         <v>74</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>282</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>283</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>74</v>
@@ -5091,13 +5118,13 @@
         <v>74</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>74</v>
@@ -5106,27 +5133,27 @@
         <v>96</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>293</v>
+        <v>257</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>74</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5134,28 +5161,28 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>295</v>
+        <v>160</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -5206,7 +5233,7 @@
         <v>74</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>75</v>
@@ -5221,27 +5248,27 @@
         <v>96</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>298</v>
+        <v>74</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>301</v>
+        <v>74</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5252,7 +5279,7 @@
         <v>75</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>74</v>
@@ -5261,16 +5288,16 @@
         <v>74</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K32" t="s" s="2">
         <v>295</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5321,13 +5348,13 @@
         <v>74</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>74</v>
@@ -5339,24 +5366,24 @@
         <v>298</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>309</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5370,22 +5397,22 @@
         <v>84</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>74</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5436,7 +5463,7 @@
         <v>74</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>75</v>
@@ -5451,27 +5478,27 @@
         <v>96</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>74</v>
+        <v>309</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>74</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5482,7 +5509,7 @@
         <v>75</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>74</v>
@@ -5491,16 +5518,16 @@
         <v>74</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5551,13 +5578,13 @@
         <v>74</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI34" t="s" s="2">
         <v>74</v>
@@ -5566,27 +5593,27 @@
         <v>96</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>74</v>
+        <v>306</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>74</v>
+        <v>315</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>74</v>
+        <v>316</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>74</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5609,17 +5636,15 @@
         <v>74</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>325</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>74</v>
@@ -5668,7 +5693,7 @@
         <v>74</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>75</v>
@@ -5683,13 +5708,13 @@
         <v>96</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>74</v>
@@ -5700,10 +5725,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5714,7 +5739,7 @@
         <v>75</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>74</v>
@@ -5726,17 +5751,15 @@
         <v>74</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>151</v>
+        <v>325</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>332</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
         <v>74</v>
@@ -5785,13 +5808,13 @@
         <v>74</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>74</v>
@@ -5800,27 +5823,27 @@
         <v>96</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>333</v>
+        <v>74</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>335</v>
+        <v>74</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>285</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5843,15 +5866,17 @@
         <v>74</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>151</v>
+        <v>330</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>332</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>333</v>
+      </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>74</v>
@@ -5900,7 +5925,7 @@
         <v>74</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>75</v>
@@ -5915,38 +5940,38 @@
         <v>96</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>74</v>
+        <v>334</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO37" t="s" s="2">
-        <v>285</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>341</v>
+        <v>74</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>74</v>
@@ -5958,15 +5983,17 @@
         <v>74</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>342</v>
+        <v>160</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>339</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>340</v>
+      </c>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>74</v>
@@ -6015,13 +6042,13 @@
         <v>74</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>74</v>
@@ -6030,27 +6057,27 @@
         <v>96</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>74</v>
+        <v>343</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO38" t="s" s="2">
-        <v>74</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6058,11 +6085,11 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G39" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="G39" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="H39" t="s" s="2">
         <v>74</v>
       </c>
@@ -6073,13 +6100,13 @@
         <v>74</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>348</v>
+        <v>160</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6130,56 +6157,56 @@
         <v>74</v>
       </c>
       <c r="AF39" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK39" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL39" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="AM39" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="AG39" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="AL39" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="AM39" t="s" s="2">
-        <v>354</v>
-      </c>
       <c r="AN39" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>355</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>74</v>
+        <v>349</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>84</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>74</v>
@@ -6188,13 +6215,13 @@
         <v>74</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>151</v>
+        <v>350</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>152</v>
+        <v>351</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>153</v>
+        <v>352</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6245,25 +6272,25 @@
         <v>74</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>154</v>
+        <v>348</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>74</v>
+        <v>353</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>155</v>
+        <v>354</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>74</v>
@@ -6277,18 +6304,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
-        <v>129</v>
+        <v>74</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>76</v>
@@ -6303,17 +6330,15 @@
         <v>74</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>130</v>
+        <v>356</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>131</v>
+        <v>357</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>133</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
         <v>74</v>
@@ -6362,10 +6387,10 @@
         <v>74</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>161</v>
+        <v>355</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>76</v>
@@ -6374,66 +6399,62 @@
         <v>74</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>135</v>
+        <v>359</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>74</v>
+        <v>360</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>74</v>
+        <v>362</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>74</v>
+        <v>363</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
-        <v>359</v>
+        <v>74</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>360</v>
+        <v>161</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>361</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="O42" t="s" s="2">
-        <v>139</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
         <v>74</v>
       </c>
@@ -6481,25 +6502,25 @@
         <v>74</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>362</v>
+        <v>163</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>135</v>
+        <v>74</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>127</v>
+        <v>164</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>74</v>
@@ -6513,14 +6534,14 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" t="s" s="2">
@@ -6536,19 +6557,19 @@
         <v>74</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>364</v>
+        <v>166</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>365</v>
+        <v>167</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>366</v>
+        <v>147</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6574,13 +6595,13 @@
         <v>74</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>178</v>
+        <v>74</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>367</v>
+        <v>74</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>368</v>
+        <v>74</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>74</v>
@@ -6598,7 +6619,7 @@
         <v>74</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>363</v>
+        <v>169</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>75</v>
@@ -6610,62 +6631,66 @@
         <v>74</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>369</v>
+        <v>164</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>155</v>
+        <v>74</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>370</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>74</v>
+        <v>367</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
         <v>75</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>74</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="J44" t="s" s="2">
         <v>85</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>372</v>
+        <v>129</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="O44" t="s" s="2">
+        <v>148</v>
+      </c>
       <c r="P44" t="s" s="2">
         <v>74</v>
       </c>
@@ -6713,42 +6738,42 @@
         <v>74</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>375</v>
+        <v>127</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>376</v>
+        <v>74</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>377</v>
+        <v>74</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>378</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6759,7 +6784,7 @@
         <v>75</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>74</v>
@@ -6771,15 +6796,17 @@
         <v>85</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>104</v>
+        <v>181</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>373</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>374</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>74</v>
@@ -6804,13 +6831,13 @@
         <v>74</v>
       </c>
       <c r="X45" t="s" s="2">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="Y45" t="s" s="2">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="Z45" t="s" s="2">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="AA45" t="s" s="2">
         <v>74</v>
@@ -6828,13 +6855,13 @@
         <v>74</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>75</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>74</v>
@@ -6846,24 +6873,24 @@
         <v>74</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>385</v>
+        <v>164</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>74</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>74</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6871,7 +6898,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>84</v>
@@ -6886,13 +6913,13 @@
         <v>85</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>104</v>
+        <v>380</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -6919,13 +6946,13 @@
         <v>74</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>167</v>
+        <v>74</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>389</v>
+        <v>74</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>390</v>
+        <v>74</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>74</v>
@@ -6943,10 +6970,10 @@
         <v>74</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>84</v>
@@ -6961,24 +6988,24 @@
         <v>74</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>74</v>
+        <v>385</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6998,16 +7025,16 @@
         <v>74</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>201</v>
+        <v>104</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7034,13 +7061,13 @@
         <v>74</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>74</v>
+        <v>390</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>74</v>
+        <v>391</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>74</v>
@@ -7058,7 +7085,7 @@
         <v>74</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>75</v>
@@ -7076,10 +7103,10 @@
         <v>74</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>155</v>
+        <v>392</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>74</v>
+        <v>393</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>74</v>
@@ -7090,10 +7117,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7101,10 +7128,10 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>74</v>
@@ -7113,20 +7140,18 @@
         <v>74</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>201</v>
+        <v>104</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>399</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>400</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
         <v>74</v>
@@ -7151,13 +7176,13 @@
         <v>74</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>74</v>
+        <v>397</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>74</v>
+        <v>398</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>74</v>
@@ -7175,13 +7200,13 @@
         <v>74</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>74</v>
@@ -7190,23 +7215,255 @@
         <v>96</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>298</v>
+        <v>74</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="AM48" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AO48" t="s" s="2">
+    </row>
+    <row r="49" hidden="true">
+      <c r="A49" t="s" s="2">
         <v>402</v>
+      </c>
+      <c r="B49" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G49" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K49" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF49" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AG49" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH49" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ49" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AL49" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AM49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN49" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO49" t="s" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" hidden="true">
+      <c r="A50" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="B50" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="G50" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="I50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="J50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q50" s="2"/>
+      <c r="R50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="S50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="T50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="V50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="W50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="X50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Z50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AA50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AB50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AC50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AD50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AE50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AF50" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AG50" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AH50" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AJ50" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK50" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="AL50" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="AM50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AN50" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="AO50" t="s" s="2">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO48">
+  <autoFilter ref="A1:AO50">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7216,7 +7473,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI47">
+  <conditionalFormatting sqref="A2:AI49">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>